<commit_message>
Adjusted folder structure and moved some files. Began work on graphs
</commit_message>
<xml_diff>
--- a/Progress_Report.xlsx
+++ b/Progress_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\visual-studio-code\java-dojo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2641EED8-4998-4F96-86FA-5F20CFC651BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8A0DA14-9B60-4A81-BDC9-46B5B974598C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="DataStructures &amp; Algorithms" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -448,7 +449,7 @@
   <dimension ref="A1:AD20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="AE10" sqref="AE10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -746,16 +747,16 @@
       <c r="D13" s="3">
         <v>167</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="3">
         <v>168</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="3">
         <v>169</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="3">
         <v>170</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="3">
         <v>171</v>
       </c>
       <c r="I13">

</xml_diff>

<commit_message>
Completed adjacencyLishGraph implementation and began binary tree implementations
</commit_message>
<xml_diff>
--- a/Progress_Report.xlsx
+++ b/Progress_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\visual-studio-code\java-dojo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8A0DA14-9B60-4A81-BDC9-46B5B974598C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4C0817-FA13-4E5E-92A3-40A6B0DB9E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="DataStructures &amp; Algorithms" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -449,7 +448,7 @@
   <dimension ref="A1:AD20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE10" sqref="AE10"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -722,8 +721,14 @@
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>102</v>
+      </c>
+      <c r="C11" s="3">
+        <v>103</v>
+      </c>
+      <c r="D11" s="3">
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.3">

</xml_diff>